<commit_message>
work on log file loading
</commit_message>
<xml_diff>
--- a/Error Codes.xlsx
+++ b/Error Codes.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdavenport/Projects/LogReview/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{36FA9B04-0E35-294D-8DDF-30A9746B2A09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A333DD99-8F2C-704F-8629-1505505DFF53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32000" yWindow="240" windowWidth="18000" windowHeight="17500" xr2:uid="{3B4ADFBF-9D50-544B-A6B1-3F01B8B2884B}"/>
+    <workbookView xWindow="32000" yWindow="240" windowWidth="18000" windowHeight="17500" activeTab="1" xr2:uid="{3B4ADFBF-9D50-544B-A6B1-3F01B8B2884B}"/>
   </bookViews>
   <sheets>
     <sheet name="backend" sheetId="1" r:id="rId1"/>
     <sheet name="appsvr" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>Error Code</t>
   </si>
@@ -74,16 +75,83 @@
   </si>
   <si>
     <t>./AOLogs/appsvr/server.log:com.ph.phoenix.ApplicationException: You have attempted to log in as administrator from an untrusted domain: 142.58.103.11</t>
+  </si>
+  <si>
+    <t>ApplicationException</t>
+  </si>
+  <si>
+    <t>You have attempted to log in as administrator from an untrusted domain</t>
+  </si>
+  <si>
+    <t>Login attempt from device on untrusted domain</t>
+  </si>
+  <si>
+    <t>Use device on trusted domain or Add host or CIDR Range to Trusted Hosts - https://help.fortinet.com/fsiem/6-6-2/Online-Help/HTML5_Help/System_Settings.htm#Trusted</t>
+  </si>
+  <si>
+    <t>ErrorID</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>SyntaxError</t>
+  </si>
+  <si>
+    <t>Unexpected token u in JSON at position 0</t>
+  </si>
+  <si>
+    <t>SyntaxError: Unexpected token u in JSON at position 0
+at JSON.parse (&lt;anonymous&gt;)
+at mergeData (/opt/node-rest-service/web/router/api/named-value/get.js:10:26)
+at module.exports (/opt/node-rest-service/web/router/api/named-value/get.js:80:17)
+at runMicrotasks (&lt;anonymous&gt;)
+at processTicksAndRejections (internal/process/task_queues.js:95:5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phRuleWorker slows or stops event ingestion when pm2/redis returns 50X apache response </t>
+  </si>
+  <si>
+    <t>6.6.2 performance patch https://mantis.fortinet.com/bug_view_page.php?bug_id=0857550</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -109,11 +177,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,119 +497,179 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CB769B5-3263-DF45-92AB-AF6AC39CCE24}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="49.5" customWidth="1"/>
-    <col min="2" max="2" width="18.1640625" customWidth="1"/>
-    <col min="3" max="3" width="61.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" customWidth="1"/>
-    <col min="5" max="5" width="28.1640625" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="49.5" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" customWidth="1"/>
+    <col min="4" max="4" width="61.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="28.1640625" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="107" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="107" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87AFFF5B-FEF3-8642-A40D-C4F2EBAE78F2}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.83203125" customWidth="1"/>
-    <col min="2" max="2" width="18.1640625" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" customWidth="1"/>
-    <col min="5" max="5" width="16.5" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16.5" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="153" x14ac:dyDescent="0.2">
-      <c r="C2" s="1" t="s">
+    <row r="2" spans="1:7" ht="187" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C4" s="1"/>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="1">
+        <v>7722497</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="372" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="2">
+        <v>7738383</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
handle backend phoenix.log better
</commit_message>
<xml_diff>
--- a/Error Codes.xlsx
+++ b/Error Codes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdavenport/Projects/LogReview/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A333DD99-8F2C-704F-8629-1505505DFF53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8470925C-F2D2-0E4C-93B7-93FC43A5BA99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32000" yWindow="240" windowWidth="18000" windowHeight="17500" activeTab="1" xr2:uid="{3B4ADFBF-9D50-544B-A6B1-3F01B8B2884B}"/>
+    <workbookView xWindow="6200" yWindow="1000" windowWidth="19400" windowHeight="17500" activeTab="1" xr2:uid="{3B4ADFBF-9D50-544B-A6B1-3F01B8B2884B}"/>
   </bookViews>
   <sheets>
     <sheet name="backend" sheetId="1" r:id="rId1"/>
@@ -499,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CB769B5-3263-DF45-92AB-AF6AC39CCE24}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>